<commit_message>
update readme and training test
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/opset_22/CPU/training_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/opset_22/CPU/training_CPUExecutionProvider.xlsx
@@ -27,7 +27,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -52,6 +52,12 @@
         <bgColor rgb="00EEEEEE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9E1F2"/>
+        <bgColor rgb="00D9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -65,11 +71,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -208,14 +215,25 @@
               </a:ln>
             </spPr>
           </dPt>
+          <dPt>
+            <idx val="3"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="4D7CFE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
           <cat>
             <numRef>
-              <f>'Data_PieChart'!$A$2:$A$4</f>
+              <f>'Data_PieChart'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Data_PieChart'!$B$2:$B$4</f>
+              <f>'Data_PieChart'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -559,7 +577,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="48" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
     <col width="100" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -616,17 +634,17 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>And</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
@@ -703,119 +721,119 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Bernoulli</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomUniformLike(22) node with name ''</t>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>BitShift</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT32).</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>BitwiseAnd</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>BitwiseNot</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>BitwiseOr</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>BitwiseXor</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>BlackmanWindow</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
@@ -834,7 +852,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::53_Grad/Sub_1).
+          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::22491_Grad/Sub_1).
 </t>
         </is>
       </c>
@@ -946,51 +964,51 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>ConcatFromSequence</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UNDEFINED).</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>Constant</t>
         </is>
       </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>Node Constant has no editable input.</t>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>ConstantOfShape</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
@@ -1014,17 +1032,17 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>ConvInteger</t>
         </is>
       </c>
-      <c r="B27" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C27" s="3" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -1085,19 +1103,19 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr">
+      <c r="A31" s="3" t="inlineStr">
         <is>
           <t>DeformConv</t>
         </is>
       </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DeformConv(22) node with name ''</t>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -1120,17 +1138,17 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>DequantizeLinear</t>
         </is>
       </c>
-      <c r="B33" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -1237,7 +1255,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::172): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22610): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1294,19 +1312,19 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="inlineStr">
+      <c r="A43" s="4" t="inlineStr">
         <is>
           <t>GRU</t>
         </is>
       </c>
-      <c r="B43" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C43" s="3" t="inlineStr">
-        <is>
-          <t>Skipping recurrent ops (GRU/LSTM)</t>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>NOT_TESTED</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>Not tested because it crash python kernel</t>
         </is>
       </c>
     </row>
@@ -1442,7 +1460,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::262): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22700): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1477,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::264): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22702): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1500,34 +1518,34 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="inlineStr">
+      <c r="A55" s="2" t="inlineStr">
         <is>
           <t>HammingWindow</t>
         </is>
       </c>
-      <c r="B55" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C55" s="3" t="inlineStr">
+      <c r="B55" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="inlineStr">
+      <c r="A56" s="2" t="inlineStr">
         <is>
           <t>HannWindow</t>
         </is>
       </c>
-      <c r="B56" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C56" s="3" t="inlineStr">
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
@@ -1605,17 +1623,17 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="3" t="inlineStr">
+      <c r="A61" s="2" t="inlineStr">
         <is>
           <t>If</t>
         </is>
       </c>
-      <c r="B61" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C61" s="3" t="inlineStr">
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
@@ -1634,7 +1652,7 @@
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got UINT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -1669,7 +1687,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::317): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22755): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1704,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::319): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22757): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1709,19 +1727,19 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="inlineStr">
+      <c r="A67" s="4" t="inlineStr">
         <is>
           <t>LSTM</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C67" s="3" t="inlineStr">
-        <is>
-          <t>Skipping recurrent ops (GRU/LSTM)</t>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>NOT_TESTED</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>Not tested because it crash python kernel</t>
         </is>
       </c>
     </row>
@@ -1755,7 +1773,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::337): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22775): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1772,41 +1790,41 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::339): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22777): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="3" t="inlineStr">
+      <c r="A71" s="2" t="inlineStr">
         <is>
           <t>Loop</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C71" s="3" t="inlineStr">
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="inlineStr">
+      <c r="A72" s="3" t="inlineStr">
         <is>
           <t>LpNormalization</t>
         </is>
       </c>
-      <c r="B72" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C72" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for LpNormalization(22) node with name ''</t>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -1846,17 +1864,17 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="3" t="inlineStr">
+      <c r="A75" s="2" t="inlineStr">
         <is>
           <t>MatMulInteger</t>
         </is>
       </c>
-      <c r="B75" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C75" s="3" t="inlineStr">
+      <c r="B75" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -1898,19 +1916,19 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="inlineStr">
+      <c r="A78" s="3" t="inlineStr">
         <is>
           <t>MaxRoiPool</t>
         </is>
       </c>
-      <c r="B78" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C78" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MaxRoiPool(22) node with name ''</t>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -1969,17 +1987,17 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="3" t="inlineStr">
+      <c r="A82" s="2" t="inlineStr">
         <is>
           <t>MelWeightMatrix</t>
         </is>
       </c>
-      <c r="B82" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C82" s="3" t="inlineStr">
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
@@ -2038,19 +2056,19 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="inlineStr">
+      <c r="A86" s="3" t="inlineStr">
         <is>
           <t>Multinomial</t>
         </is>
       </c>
-      <c r="B86" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Multinomial(22) node with name ''</t>
+      <c r="B86" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C86" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -2108,51 +2126,51 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="3" t="inlineStr">
+      <c r="A90" s="2" t="inlineStr">
         <is>
           <t>Not</t>
         </is>
       </c>
-      <c r="B90" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C90" s="3" t="inlineStr">
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="3" t="inlineStr">
+      <c r="A91" s="2" t="inlineStr">
         <is>
           <t>Not</t>
         </is>
       </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C91" s="3" t="inlineStr">
+      <c r="B91" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="3" t="inlineStr">
+      <c r="A92" s="2" t="inlineStr">
         <is>
           <t>OneHot</t>
         </is>
       </c>
-      <c r="B92" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C92" s="3" t="inlineStr">
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
@@ -2171,7 +2189,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::435): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::22873): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2229,17 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="3" t="inlineStr">
+      <c r="A96" s="2" t="inlineStr">
         <is>
           <t>Or</t>
         </is>
       </c>
-      <c r="B96" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C96" s="3" t="inlineStr">
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
@@ -2280,34 +2298,34 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="3" t="inlineStr">
+      <c r="A100" s="2" t="inlineStr">
         <is>
           <t>QLinearConv</t>
         </is>
       </c>
-      <c r="B100" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C100" s="3" t="inlineStr">
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="3" t="inlineStr">
+      <c r="A101" s="2" t="inlineStr">
         <is>
           <t>QLinearMatMul</t>
         </is>
       </c>
-      <c r="B101" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C101" s="3" t="inlineStr">
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -2326,7 +2344,7 @@
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::472): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::22910): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -2349,70 +2367,70 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="inlineStr">
+      <c r="A104" s="3" t="inlineStr">
         <is>
           <t>RandomNormal</t>
         </is>
       </c>
-      <c r="B104" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C104" s="2" t="inlineStr">
-        <is>
-          <t>Node RandomNormal has no editable input.</t>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="inlineStr">
+      <c r="A105" s="3" t="inlineStr">
         <is>
           <t>RandomNormalLike</t>
         </is>
       </c>
-      <c r="B105" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C105" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomNormalLike(22) node with name ''</t>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="inlineStr">
+      <c r="A106" s="3" t="inlineStr">
         <is>
           <t>RandomUniform</t>
         </is>
       </c>
-      <c r="B106" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C106" s="2" t="inlineStr">
-        <is>
-          <t>Node RandomUniform has no editable input.</t>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="inlineStr">
+      <c r="A107" s="3" t="inlineStr">
         <is>
           <t>RandomUniformLike</t>
         </is>
       </c>
-      <c r="B107" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C107" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomUniformLike(22) node with name ''</t>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -2610,17 +2628,17 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="3" t="inlineStr">
+      <c r="A119" s="2" t="inlineStr">
         <is>
           <t>RegexFullMatch</t>
         </is>
       </c>
-      <c r="B119" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C119" s="3" t="inlineStr">
+      <c r="B119" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C119" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
@@ -2680,19 +2698,19 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="inlineStr">
+      <c r="A123" s="3" t="inlineStr">
         <is>
           <t>RoiAlign</t>
         </is>
       </c>
-      <c r="B123" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C123" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RoiAlign(22) node with name ''</t>
+      <c r="B123" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C123" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -2870,37 +2888,36 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="3" t="inlineStr">
+      <c r="A134" s="2" t="inlineStr">
         <is>
           <t>SequenceMap</t>
         </is>
       </c>
-      <c r="B134" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C134" s="3" t="inlineStr">
+      <c r="B134" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C134" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UNDEFINED).</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="inlineStr">
+      <c r="A135" s="3" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="B135" s="2" t="inlineStr">
-        <is>
-          <t>FAIL training</t>
-        </is>
-      </c>
-      <c r="C135" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\core\framework\gradient_graph_builder.cc:141 onnxruntime::training::GradientGraphBuilder::GradientGraphBuilder __train_C couldn't find the consumer node.
-</t>
+      <c r="B135" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C135" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3028,51 +3045,51 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="3" t="inlineStr">
+      <c r="A143" s="2" t="inlineStr">
         <is>
           <t>StringConcat</t>
         </is>
       </c>
-      <c r="B143" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C143" s="3" t="inlineStr">
+      <c r="B143" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C143" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="3" t="inlineStr">
+      <c r="A144" s="2" t="inlineStr">
         <is>
           <t>StringNormalizer</t>
         </is>
       </c>
-      <c r="B144" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C144" s="3" t="inlineStr">
+      <c r="B144" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C144" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="3" t="inlineStr">
+      <c r="A145" s="2" t="inlineStr">
         <is>
           <t>StringSplit</t>
         </is>
       </c>
-      <c r="B145" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C145" s="3" t="inlineStr">
+      <c r="B145" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C145" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
@@ -3114,17 +3131,17 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="3" t="inlineStr">
+      <c r="A148" s="2" t="inlineStr">
         <is>
           <t>TfIdfVectorizer</t>
         </is>
       </c>
-      <c r="B148" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C148" s="3" t="inlineStr">
+      <c r="B148" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C148" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
@@ -3199,17 +3216,17 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="3" t="inlineStr">
+      <c r="A153" s="2" t="inlineStr">
         <is>
           <t>Unique</t>
         </is>
       </c>
-      <c r="B153" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C153" s="3" t="inlineStr">
+      <c r="B153" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C153" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
@@ -3233,34 +3250,34 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="3" t="inlineStr">
+      <c r="A155" s="2" t="inlineStr">
         <is>
           <t>Where</t>
         </is>
       </c>
-      <c r="B155" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C155" s="3" t="inlineStr">
+      <c r="B155" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C155" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="3" t="inlineStr">
+      <c r="A156" s="2" t="inlineStr">
         <is>
           <t>Xor</t>
         </is>
       </c>
-      <c r="B156" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C156" s="3" t="inlineStr">
+      <c r="B156" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C156" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
@@ -3285,53 +3302,53 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="3" t="inlineStr">
+      <c r="A158" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.BeamSearch</t>
         </is>
       </c>
-      <c r="B158" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C158" s="3" t="inlineStr">
+      <c r="B158" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C158" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="2" t="inlineStr">
+      <c r="A159" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.BiasAdd</t>
         </is>
       </c>
-      <c r="B159" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C159" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasAdd(1) node with name ''</t>
+      <c r="B159" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C159" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="2" t="inlineStr">
+      <c r="A160" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.BiasDropout</t>
         </is>
       </c>
-      <c r="B160" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C160" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasDropout(1) node with name ''</t>
+      <c r="B160" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C160" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3353,87 +3370,87 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="inlineStr">
+      <c r="A162" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.BiasSoftmax</t>
         </is>
       </c>
-      <c r="B162" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C162" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSoftmax(1) node with name ''</t>
+      <c r="B162" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C162" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="2" t="inlineStr">
+      <c r="A163" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.BiasSplitGelu</t>
         </is>
       </c>
-      <c r="B163" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C163" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSplitGelu(1) node with name ''</t>
+      <c r="B163" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C163" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="3" t="inlineStr">
+      <c r="A164" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.BifurcationDetector</t>
         </is>
       </c>
-      <c r="B164" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C164" s="3" t="inlineStr">
+      <c r="B164" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C164" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="inlineStr">
+      <c r="A165" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.BitmaskBiasDropout</t>
         </is>
       </c>
-      <c r="B165" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C165" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskBiasDropout(1) node with name ''</t>
+      <c r="B165" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C165" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="2" t="inlineStr">
+      <c r="A166" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.BitmaskDropout</t>
         </is>
       </c>
-      <c r="B166" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C166" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskDropout(1) node with name ''</t>
+      <c r="B166" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C166" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3456,36 +3473,36 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="2" t="inlineStr">
+      <c r="A168" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.ComplexMul</t>
         </is>
       </c>
-      <c r="B168" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C168" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMul(1) node with name ''</t>
+      <c r="B168" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C168" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="2" t="inlineStr">
+      <c r="A169" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.ComplexMulConj</t>
         </is>
       </c>
-      <c r="B169" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C169" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMulConj(1) node with name ''</t>
+      <c r="B169" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C169" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3526,19 +3543,19 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="inlineStr">
+      <c r="A172" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.DecoderAttention</t>
         </is>
       </c>
-      <c r="B172" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C172" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DecoderAttention(1) node with name ''</t>
+      <c r="B172" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C172" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3561,19 +3578,19 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="2" t="inlineStr">
+      <c r="A174" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.DecoderMaskedSelfAttention</t>
         </is>
       </c>
-      <c r="B174" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C174" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", com.microsoft.DecoderMaskedSelfAttention, "", -1) : ("X_scaled": tensor(float),) -&gt; ("Y": tensor(float),) , Error No Op registered for com.microsoft.DecoderMaskedSelfAttention with domain_version of 22</t>
+      <c r="B174" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C174" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3590,22 +3607,22 @@
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got UINT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="3" t="inlineStr">
+      <c r="A176" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.DequantizeLinear</t>
         </is>
       </c>
-      <c r="B176" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C176" s="3" t="inlineStr">
+      <c r="B176" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C176" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -3624,7 +3641,7 @@
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3683,17 +3700,17 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="3" t="inlineStr">
+      <c r="A181" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.EmbedLayerNormalization</t>
         </is>
       </c>
-      <c r="B181" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C181" s="3" t="inlineStr">
+      <c r="B181" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C181" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
@@ -3789,36 +3806,36 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="2" t="inlineStr">
+      <c r="A187" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.FusedMatMulActivation</t>
         </is>
       </c>
-      <c r="B187" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C187" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for FusedMatMulActivation(1) node with name ''</t>
+      <c r="B187" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C187" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="2" t="inlineStr">
+      <c r="A188" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.GatedRelativePositionBias</t>
         </is>
       </c>
-      <c r="B188" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C188" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GatedRelativePositionBias(1) node with name ''</t>
+      <c r="B188" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C188" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3835,7 +3852,7 @@
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got UINT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3874,53 +3891,53 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="2" t="inlineStr">
+      <c r="A192" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.GemmFastGelu</t>
         </is>
       </c>
-      <c r="B192" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C192" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFastGelu(1) node with name ''</t>
+      <c r="B192" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C192" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="2" t="inlineStr">
+      <c r="A193" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.GemmFloat8</t>
         </is>
       </c>
-      <c r="B193" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C193" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFloat8(1) node with name ''</t>
+      <c r="B193" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C193" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="2" t="inlineStr">
+      <c r="A194" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.GemmaRotaryEmbedding</t>
         </is>
       </c>
-      <c r="B194" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C194" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_q) of operator (GemmaRotaryEmbedding) in node () is invalid.</t>
+      <c r="B194" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C194" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3937,7 +3954,7 @@
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT32).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -3960,19 +3977,19 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="2" t="inlineStr">
+      <c r="A197" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.GroupNorm</t>
         </is>
       </c>
-      <c r="B197" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C197" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GroupNorm(1) node with name ''</t>
+      <c r="B197" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C197" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4013,36 +4030,36 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="2" t="inlineStr">
+      <c r="A200" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.Irfft</t>
         </is>
       </c>
-      <c r="B200" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C200" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Irfft(1) node with name ''</t>
+      <c r="B200" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C200" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="2" t="inlineStr">
+      <c r="A201" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.LongformerAttention</t>
         </is>
       </c>
-      <c r="B201" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C201" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for LongformerAttention(1) node with name ''</t>
+      <c r="B201" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C201" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4064,52 +4081,51 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="2" t="inlineStr">
+      <c r="A203" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.MatMulFpQ4</t>
         </is>
       </c>
-      <c r="B203" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C203" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Non-zero status code returned while running MatMulFpQ4 node. Name:'' Status Message: C:\Users\COCO\onnxruntime_training_cuda_python\onnxruntime\contrib_ops\cpu\matmul_fpq4.cc:55 onnxruntime::contrib::MatMulFpQ4::Compute buf_size &gt; 0 was false. Operator MatMulFpQ4 not yet supported on this hardware platform.
-</t>
+      <c r="B203" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C203" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="3" t="inlineStr">
+      <c r="A204" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.MatMulInteger16</t>
         </is>
       </c>
-      <c r="B204" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C204" s="3" t="inlineStr">
+      <c r="B204" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C204" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT16).</t>
         </is>
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="3" t="inlineStr">
+      <c r="A205" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.MatMulIntegerToFloat</t>
         </is>
       </c>
-      <c r="B205" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C205" s="3" t="inlineStr">
+      <c r="B205" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C205" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT8).</t>
         </is>
@@ -4152,36 +4168,36 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="2" t="inlineStr">
+      <c r="A208" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.MoE</t>
         </is>
       </c>
-      <c r="B208" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C208" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MoE(1) node with name ''</t>
+      <c r="B208" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C208" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="2" t="inlineStr">
+      <c r="A209" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.MulInteger</t>
         </is>
       </c>
-      <c r="B209" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C209" s="2" t="inlineStr">
-        <is>
-          <t>Node Constant has no editable input.</t>
+      <c r="B209" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C209" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4204,121 +4220,121 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="3" t="inlineStr">
+      <c r="A211" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.MurmurHash3</t>
         </is>
       </c>
-      <c r="B211" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C211" s="3" t="inlineStr">
+      <c r="B211" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C211" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="3" t="inlineStr">
+      <c r="A212" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.NGramRepeatBlock</t>
         </is>
       </c>
-      <c r="B212" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C212" s="3" t="inlineStr">
+      <c r="B212" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C212" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT64).</t>
         </is>
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="2" t="inlineStr">
+      <c r="A213" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.NhwcConv</t>
         </is>
       </c>
-      <c r="B213" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C213" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for NhwcConv(1) node with name ''</t>
+      <c r="B213" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C213" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="2" t="inlineStr">
+      <c r="A214" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.NhwcFusedConv</t>
         </is>
       </c>
-      <c r="B214" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C214" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_X_fp16) of operator (NhwcFusedConv) in node () is invalid.</t>
+      <c r="B214" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C214" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="3" t="inlineStr">
+      <c r="A215" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.NhwcMaxPool</t>
         </is>
       </c>
-      <c r="B215" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C215" s="3" t="inlineStr">
+      <c r="B215" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C215" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="2" t="inlineStr">
+      <c r="A216" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.PackedAttention</t>
         </is>
       </c>
-      <c r="B216" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C216" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedAttention(1) node with name ''</t>
+      <c r="B216" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C216" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="2" t="inlineStr">
+      <c r="A217" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.PackedMultiHeadAttention</t>
         </is>
       </c>
-      <c r="B217" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C217" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedMultiHeadAttention(1) node with name ''</t>
+      <c r="B217" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C217" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4340,68 +4356,68 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="3" t="inlineStr">
+      <c r="A219" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QAttention</t>
         </is>
       </c>
-      <c r="B219" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C219" s="3" t="inlineStr">
+      <c r="B219" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C219" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="3" t="inlineStr">
+      <c r="A220" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QGemm</t>
         </is>
       </c>
-      <c r="B220" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C220" s="3" t="inlineStr">
+      <c r="B220" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C220" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="3" t="inlineStr">
+      <c r="A221" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearAdd</t>
         </is>
       </c>
-      <c r="B221" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C221" s="3" t="inlineStr">
+      <c r="B221" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C221" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="3" t="inlineStr">
+      <c r="A222" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearAveragePool</t>
         </is>
       </c>
-      <c r="B222" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C222" s="3" t="inlineStr">
+      <c r="B222" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C222" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -4420,73 +4436,73 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::929): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::23360): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="3" t="inlineStr">
+      <c r="A224" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearConv</t>
         </is>
       </c>
-      <c r="B224" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C224" s="3" t="inlineStr">
+      <c r="B224" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C224" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="3" t="inlineStr">
+      <c r="A225" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearGlobalAveragePool</t>
         </is>
       </c>
-      <c r="B225" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C225" s="3" t="inlineStr">
+      <c r="B225" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C225" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="3" t="inlineStr">
+      <c r="A226" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearLeakyRelu</t>
         </is>
       </c>
-      <c r="B226" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C226" s="3" t="inlineStr">
+      <c r="B226" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C226" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="3" t="inlineStr">
+      <c r="A227" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearMul</t>
         </is>
       </c>
-      <c r="B227" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C227" s="3" t="inlineStr">
+      <c r="B227" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C227" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
@@ -4505,75 +4521,75 @@
       </c>
       <c r="C228" s="3" t="inlineStr">
         <is>
+          <t>Training not attempted: inference FAIL</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearSigmoid</t>
+        </is>
+      </c>
+      <c r="B229" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C229" s="2" t="inlineStr">
+        <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
-    <row r="229">
-      <c r="A229" s="3" t="inlineStr">
-        <is>
-          <t>com.microsoft.QLinearSigmoid</t>
-        </is>
-      </c>
-      <c r="B229" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C229" s="3" t="inlineStr">
+    <row r="230">
+      <c r="A230" s="2" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearSoftmax</t>
+        </is>
+      </c>
+      <c r="B230" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C230" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UINT8).</t>
         </is>
       </c>
     </row>
-    <row r="230">
-      <c r="A230" s="3" t="inlineStr">
-        <is>
-          <t>com.microsoft.QLinearSoftmax</t>
-        </is>
-      </c>
-      <c r="B230" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C230" s="3" t="inlineStr">
-        <is>
-          <t>Training scaling unsupported for non-float first input (got UINT8).</t>
-        </is>
-      </c>
-    </row>
     <row r="231">
-      <c r="A231" s="3" t="inlineStr">
+      <c r="A231" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.QLinearWhere</t>
         </is>
       </c>
-      <c r="B231" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C231" s="3" t="inlineStr">
+      <c r="B231" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C231" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got BOOL).</t>
         </is>
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="2" t="inlineStr">
+      <c r="A232" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.QMoE</t>
         </is>
       </c>
-      <c r="B232" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C232" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Mul) bound to different types (tensor(float16) and tensor(float) in node ().</t>
+      <c r="B232" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C232" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4590,7 +4606,7 @@
       </c>
       <c r="C233" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4607,7 +4623,7 @@
       </c>
       <c r="C234" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4624,7 +4640,7 @@
       </c>
       <c r="C235" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4641,7 +4657,7 @@
       </c>
       <c r="C236" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4658,24 +4674,24 @@
       </c>
       <c r="C237" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="2" t="inlineStr">
+      <c r="A238" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.QuantizeBFP</t>
         </is>
       </c>
-      <c r="B238" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C238" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeBFP(1) node with name ''</t>
+      <c r="B238" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C238" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4692,24 +4708,24 @@
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::934): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::23365): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="2" t="inlineStr">
+      <c r="A240" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.QuantizeWithOrder</t>
         </is>
       </c>
-      <c r="B240" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C240" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeWithOrder(1) node with name ''</t>
+      <c r="B240" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C240" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4731,17 +4747,17 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="3" t="inlineStr">
+      <c r="A242" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.Range</t>
         </is>
       </c>
-      <c r="B242" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C242" s="3" t="inlineStr">
+      <c r="B242" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C242" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
@@ -4760,75 +4776,75 @@
       </c>
       <c r="C243" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT8).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="2" t="inlineStr">
+      <c r="A244" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.RelativePositionBias</t>
         </is>
       </c>
-      <c r="B244" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C244" s="2" t="inlineStr">
-        <is>
-          <t>Cannot find graph.input for 'bias_table'.</t>
+      <c r="B244" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C244" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="2" t="inlineStr">
+      <c r="A245" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.RemovePadding</t>
         </is>
       </c>
-      <c r="B245" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C245" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RemovePadding(1) node with name ''</t>
+      <c r="B245" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C245" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="2" t="inlineStr">
+      <c r="A246" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.RestorePadding</t>
         </is>
       </c>
-      <c r="B246" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C246" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RestorePadding(1) node with name ''</t>
+      <c r="B246" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C246" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="2" t="inlineStr">
+      <c r="A247" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.Rfft</t>
         </is>
       </c>
-      <c r="B247" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C247" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Rfft(1) node with name ''</t>
+      <c r="B247" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C247" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4869,36 +4885,36 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="3" t="inlineStr">
+      <c r="A250" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.Sampling</t>
         </is>
       </c>
-      <c r="B250" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C250" s="3" t="inlineStr">
+      <c r="B250" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C250" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got INT32).</t>
         </is>
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="2" t="inlineStr">
+      <c r="A251" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.SkipGroupNorm</t>
         </is>
       </c>
-      <c r="B251" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C251" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for SkipGroupNorm(1) node with name ''</t>
+      <c r="B251" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C251" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4939,19 +4955,19 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="2" t="inlineStr">
+      <c r="A254" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.Snpe</t>
         </is>
       </c>
-      <c r="B254" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C254" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Snpe(1) node with name ''</t>
+      <c r="B254" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C254" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -4973,53 +4989,53 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="3" t="inlineStr">
+      <c r="A256" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.SparseToDenseMatMul</t>
         </is>
       </c>
-      <c r="B256" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C256" s="3" t="inlineStr">
+      <c r="B256" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C256" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got UNDEFINED).</t>
         </is>
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="3" t="inlineStr">
+      <c r="A257" s="2" t="inlineStr">
         <is>
           <t>com.microsoft.Tokenizer</t>
         </is>
       </c>
-      <c r="B257" s="3" t="inlineStr">
-        <is>
-          <t>SKIPPED</t>
-        </is>
-      </c>
-      <c r="C257" s="3" t="inlineStr">
+      <c r="B257" s="2" t="inlineStr">
+        <is>
+          <t>FAIL not implemented</t>
+        </is>
+      </c>
+      <c r="C257" s="2" t="inlineStr">
         <is>
           <t>Training scaling unsupported for non-float first input (got STRING).</t>
         </is>
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="2" t="inlineStr">
+      <c r="A258" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.TorchEmbedding</t>
         </is>
       </c>
-      <c r="B258" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C258" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for TorchEmbedding(1) node with name ''</t>
+      <c r="B258" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C258" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -5089,26 +5105,24 @@
       </c>
       <c r="C262" s="3" t="inlineStr">
         <is>
-          <t>Training scaling unsupported for non-float first input (got INT32).</t>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="2" t="inlineStr">
+      <c r="A263" s="3" t="inlineStr">
         <is>
           <t>com.microsoft.WhisperBeamSearch</t>
         </is>
       </c>
-      <c r="B263" s="2" t="inlineStr">
-        <is>
-          <t>FAIL model gen</t>
-        </is>
-      </c>
-      <c r="C263" s="2" t="inlineStr">
-        <is>
-          <t>[ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", WhisperBeamSearch, "com.microsoft", -1) : ("encoder_input_ids_scaled": tensor(float),"max_length": tensor(int32),"min_length": tensor(int32),"num_beams": tensor(int32),"num_return_sequences": tensor(int32),"length_penalty": tensor(float),"repetition_penalty": tensor(float),"vocab_mask": tensor(int32),"prefix_vocab_mask": tensor(int32),"attention_mask": tensor(int32),) -&gt; ("sequences": tensor(int32),) , Error Nodes in a graph must be topologically sorted, however input 'shape4D_pass' of node: 
-name:  OpType: ConstantOfShape
- is not output of any previous nodes.</t>
+      <c r="B263" s="3" t="inlineStr">
+        <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="C263" s="3" t="inlineStr">
+        <is>
+          <t>Training not attempted: inference FAIL</t>
         </is>
       </c>
     </row>
@@ -5124,7 +5138,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5169,10 +5183,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -5182,10 +5196,23 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C4" t="n">
-        <v>27.1</v>
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NOT_TESTED</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix readme pie chart
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/opset_22/CPU/training_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/opset_22/CPU/training_CPUExecutionProvider.xlsx
@@ -852,7 +852,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::53_Grad/Sub_1).
+          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::24062_Grad/Sub_1).
 </t>
         </is>
       </c>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::172): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24181): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::262): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24271): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::264): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24273): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::317): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24326): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::319): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24328): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::337): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24346): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::339): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24348): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::435): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24444): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::472): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::24481): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::922): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::24931): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4708,7 +4708,7 @@
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::927): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::24936): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
try fixing pie chart size
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/opset_22/CPU/training_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/opset_22/CPU/training_CPUExecutionProvider.xlsx
@@ -852,7 +852,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::24062_Grad/Sub_1).
+          <t xml:space="preserve">C:\Users\COCO\onnxruntime_training_cuda_python\orttraining\orttraining\python\orttraining_pybind_state.cc:621 onnxruntime::python::addObjectMethodsForTraining::&lt;lambda_6dd399ad6691adab5d0e0423ed8ce22d&gt;::operator () [ONNXRuntimeError] : 1 : FAIL : Type Error: Type parameter (T) of Optype (Sub) bound to different types (tensor(float) and tensor(double) in node (onnx::Pow::27433_Grad/Sub_1).
 </t>
         </is>
       </c>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24181): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27552): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24271): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27642): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24273): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27644): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24326): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27697): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24328): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27699): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24346): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27717): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24348): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27719): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::24444): A typestr: T, has unsupported type: tensor(bool)</t>
+          <t>[ShapeInferenceError] (op_type:Sub, node name: onnx::Sub::27815): A typestr: T, has unsupported type: tensor(bool)</t>
         </is>
       </c>
     </row>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::24481): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::27852): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="C223" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::24931): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::28302): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>
@@ -4708,7 +4708,7 @@
       </c>
       <c r="C239" s="2" t="inlineStr">
         <is>
-          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::24936): X typestr: T, has unsupported type: tensor(uint8)</t>
+          <t>[ShapeInferenceError] (op_type:Pow, node name: onnx::Pow::28307): X typestr: T, has unsupported type: tensor(uint8)</t>
         </is>
       </c>
     </row>

</xml_diff>